<commit_message>
Complete LP5 Design and build tabular models
</commit_message>
<xml_diff>
--- a/Certification.xlsx
+++ b/Certification.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github.com\open-word\DP-600-Fabric-Analytics-Engineer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F784A69-FD85-4E15-8C8A-A1185B889F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA26116-6665-4BCE-92E7-B9CB98F6793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1680" windowWidth="29040" windowHeight="16440" xr2:uid="{C91A3575-F826-4DBB-9127-8E0D5980857F}"/>
   </bookViews>
   <sheets>
-    <sheet name="2 net" sheetId="2" r:id="rId1"/>
-    <sheet name="1 live" sheetId="1" r:id="rId2"/>
+    <sheet name=".co.uk" sheetId="3" r:id="rId1"/>
+    <sheet name=".net" sheetId="2" r:id="rId2"/>
+    <sheet name="live.co.uk" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2 net'!$B$4:$K$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'.co.uk'!$B$4:$K$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'.net'!$B$4:$J$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="120">
   <si>
     <t>Learning Path</t>
   </si>
@@ -366,9 +368,6 @@
     <t>TO DO</t>
   </si>
   <si>
-    <t>Video</t>
-  </si>
-  <si>
     <t>Learn Live</t>
   </si>
   <si>
@@ -376,16 +375,40 @@
   </si>
   <si>
     <t>PL-300 Lab 05</t>
+  </si>
+  <si>
+    <t>Choose a Power BI model framework</t>
+  </si>
+  <si>
+    <t>Referenced in "Understand scalability in Power BI"</t>
+  </si>
+  <si>
+    <t>Ep3: Work with Delta Lake tables in Microsoft Fabric</t>
+  </si>
+  <si>
+    <t>Ep2: Use Apache Spark in Microsoft Fabric</t>
+  </si>
+  <si>
+    <t>Ep1: Get started with end-to-end analytics and lakehouses in Microsoft Fabric</t>
+  </si>
+  <si>
+    <t>Ep4: Use Data Factory Pipelines in Microsoft Fabric</t>
+  </si>
+  <si>
+    <t>DUP</t>
+  </si>
+  <si>
+    <t>Ep5: Ingest Data with Dataflows Gen2 in Microsoft Fabric</t>
+  </si>
+  <si>
+    <t>Ep6: Get started with data warehouses in Microsoft Fabric</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,7 +439,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,12 +572,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -579,14 +609,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -899,10 +940,1155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F180EED-F52E-41D2-8301-1E47E800243C}">
-  <dimension ref="B2:K43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CC8F1D-AB2E-48D2-9DC5-EB07BF29C76C}">
+  <dimension ref="B2:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="71.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="K31" s="36"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="38"/>
+      <c r="C32" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J32" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="40"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="38"/>
+      <c r="C33" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="I33" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J33" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="K33" s="40"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="43"/>
+      <c r="C34" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J34" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="K34" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B4:K34" xr:uid="{3F180EED-F52E-41D2-8301-1E47E800243C}"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{08FC8A4A-0C8B-45DA-9EC0-5D2087207700}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{50714AA2-4D85-472C-9B53-394F40185DA2}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{A30204E0-8F5D-4F7D-8DF7-C54C9CF0D637}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{7788B396-D903-4148-869C-394CE8E5E0AC}"/>
+    <hyperlink ref="B23" r:id="rId5" xr:uid="{551B6BE4-8CC7-4CD9-993F-CAE042E93C52}"/>
+    <hyperlink ref="B28" r:id="rId6" display="Manage the anlytics development lifecycle" xr:uid="{294699F5-0425-4E5E-BE19-5F5797B3CFAA}"/>
+    <hyperlink ref="B19" r:id="rId7" xr:uid="{E7D00C4B-F270-4816-95E1-4EB97F6E2DFE}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{828C58D5-7883-4D4B-A57E-DA485D6B8226}"/>
+    <hyperlink ref="H4" r:id="rId9" xr:uid="{9D812F63-D687-4DA4-AC03-C5871F50BB7F}"/>
+    <hyperlink ref="I4" r:id="rId10" xr:uid="{AF29494B-B26D-4DB3-8942-219C16F81BF2}"/>
+    <hyperlink ref="J4" r:id="rId11" xr:uid="{6A15B054-F734-4491-A54E-89E8F37A8994}"/>
+    <hyperlink ref="C31" r:id="rId12" xr:uid="{A9D7A016-9658-4B6D-AE47-187DDED573FD}"/>
+    <hyperlink ref="C34" r:id="rId13" xr:uid="{557AECA1-A68C-4A38-8A65-54BEF8F993CB}"/>
+    <hyperlink ref="C33" r:id="rId14" xr:uid="{57B1034E-E8BF-4E52-8354-646733FCF9A4}"/>
+    <hyperlink ref="F4" r:id="rId15" xr:uid="{44B779E0-1056-4773-9799-C45DDC5B6F14}"/>
+    <hyperlink ref="C41" r:id="rId16" display="DP-500" xr:uid="{394898ED-3556-4EBE-BE73-0A7B04E82A8C}"/>
+    <hyperlink ref="C42" r:id="rId17" display="DP-500 GitHub Pages" xr:uid="{8ABC9B84-9D6B-4E0E-9BBC-8861EA315C0E}"/>
+    <hyperlink ref="D20" r:id="rId18" xr:uid="{34CCA4D7-8A66-4091-98C9-1826FF0630DF}"/>
+    <hyperlink ref="D21" r:id="rId19" xr:uid="{8E646F58-9C6C-48C5-84F4-A69B8BBA1C73}"/>
+    <hyperlink ref="D19" r:id="rId20" xr:uid="{1EF8D2CA-52C5-48CF-A4FB-32776BBF0D7F}"/>
+    <hyperlink ref="D27" r:id="rId21" xr:uid="{3D251DB3-E39B-427E-8F0D-B21486FAD1A5}"/>
+    <hyperlink ref="D22" r:id="rId22" xr:uid="{F24EB732-EA82-458E-AF93-19C7D2B49C95}"/>
+    <hyperlink ref="D26" r:id="rId23" xr:uid="{0BA3130C-B53F-4D96-935C-41E081EC8C5E}"/>
+    <hyperlink ref="D23" r:id="rId24" xr:uid="{86066C0B-071A-454D-AAD8-0F158D1F9AEA}"/>
+    <hyperlink ref="C44" r:id="rId25" xr:uid="{C51CD2A9-2419-4511-ADE3-9F7FE5B2E900}"/>
+    <hyperlink ref="D24" r:id="rId26" xr:uid="{0E3F65DC-9D34-4657-BB39-A4C6C9DE1C5B}"/>
+    <hyperlink ref="C45" r:id="rId27" xr:uid="{FC227DE1-3E6F-4058-91B9-6DB68B5FE69F}"/>
+    <hyperlink ref="C38" r:id="rId28" display="MSLearn Fabric (Git repository)" xr:uid="{6CBAD373-EC0A-4C4C-8753-DE9D00DD2A27}"/>
+    <hyperlink ref="C39" r:id="rId29" display="MSLearn Fabric (GitHub pages)" xr:uid="{67488736-85D0-4941-A9EB-8A6AF61E6792}"/>
+    <hyperlink ref="D25" r:id="rId30" xr:uid="{65CBD0AA-66B9-44A2-8BF7-A45177915E43}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{BFEE07C7-3F6D-42B7-8D26-6E208934F827}"/>
+    <hyperlink ref="C28" r:id="rId32" xr:uid="{37C633E2-8900-4808-9C38-C745B41EB568}"/>
+    <hyperlink ref="C29" r:id="rId33" xr:uid="{0F39F4F6-AD89-42F7-A700-9257FEF5B901}"/>
+    <hyperlink ref="C30" r:id="rId34" xr:uid="{02DBA142-08B2-47DA-A60A-BA1635B23EA1}"/>
+    <hyperlink ref="D30" r:id="rId35" xr:uid="{925A3BF1-3411-486D-8729-B1B2A4898B3C}"/>
+    <hyperlink ref="D34" r:id="rId36" display="MSLearn Fabric Lab 11" xr:uid="{A4D5207D-57D6-400A-94DA-36A14F978784}"/>
+    <hyperlink ref="D32" r:id="rId37" display="MSLearn Fabric Lab 08" xr:uid="{924A6954-B099-4A77-A65E-10DC8F72176A}"/>
+    <hyperlink ref="D31" r:id="rId38" display="MSLearn Fabric Lab 07" xr:uid="{55B490C3-F4AD-4796-95F9-D759410AFCAA}"/>
+    <hyperlink ref="C5" r:id="rId39" xr:uid="{0780142E-7343-4DCD-AB92-008EAF762216}"/>
+    <hyperlink ref="C6" r:id="rId40" xr:uid="{95ED1E52-2DA7-4DF6-9F84-80A8C766DA05}"/>
+    <hyperlink ref="C7" r:id="rId41" xr:uid="{539D57D5-C211-4A0C-92D2-2999A71BB6BE}"/>
+    <hyperlink ref="D5" r:id="rId42" xr:uid="{96C7ED78-6B14-4EEC-82A8-35A9B415E213}"/>
+    <hyperlink ref="D6" r:id="rId43" xr:uid="{EC672BCE-C045-4701-97FA-47B47D7F574C}"/>
+    <hyperlink ref="D7" r:id="rId44" xr:uid="{85092EC6-EEA8-4F83-9503-8AC052D5C418}"/>
+    <hyperlink ref="C9" r:id="rId45" xr:uid="{5A67EBDA-8F72-4F69-BBFD-E51C64188E87}"/>
+    <hyperlink ref="C8" r:id="rId46" xr:uid="{60289D9F-AF10-46C7-AC8E-1F526245EA36}"/>
+    <hyperlink ref="C10" r:id="rId47" xr:uid="{ABAC4775-46D5-4CA9-9E28-5D9F12DDAF99}"/>
+    <hyperlink ref="C11" r:id="rId48" xr:uid="{08FF5672-16AE-4258-8619-460D32897DB8}"/>
+    <hyperlink ref="C12" r:id="rId49" xr:uid="{75ABD2C1-F4B7-4F1D-A6CD-DA543F09F955}"/>
+    <hyperlink ref="C13" r:id="rId50" xr:uid="{62CF8B04-A944-428E-9EF5-2207077477C9}"/>
+    <hyperlink ref="C14" r:id="rId51" xr:uid="{0384B246-DBF9-417D-B51B-1EC53320D606}"/>
+    <hyperlink ref="C15" r:id="rId52" xr:uid="{E6814B8D-C959-4100-94EB-8D0C918777B3}"/>
+    <hyperlink ref="C16" r:id="rId53" xr:uid="{E5C88BA5-3D54-4476-9D23-8EE01BC10B57}"/>
+    <hyperlink ref="C17" r:id="rId54" xr:uid="{4BA618DB-E73A-4920-BFA7-8DC0E2CDB8CA}"/>
+    <hyperlink ref="C18" r:id="rId55" xr:uid="{14984553-9FC9-475A-8427-F5D05CDD280D}"/>
+    <hyperlink ref="C19" r:id="rId56" xr:uid="{6BD42B1B-89CC-46FD-813D-DCA8D91AC78C}"/>
+    <hyperlink ref="C20" r:id="rId57" xr:uid="{EE206722-3EEE-4582-ACF8-F01AD666611A}"/>
+    <hyperlink ref="C21" r:id="rId58" xr:uid="{17CD9ABF-CD31-4851-BA83-DEC11CEC550E}"/>
+    <hyperlink ref="C22" r:id="rId59" xr:uid="{2544FAD4-983E-4167-91D1-32D46031F07D}"/>
+    <hyperlink ref="C24" r:id="rId60" xr:uid="{4E1D200F-99F8-4FD3-8D76-2BB4904F6198}"/>
+    <hyperlink ref="C25" r:id="rId61" xr:uid="{15A21BA2-F59E-4CF6-B0D6-C28F352306F2}"/>
+    <hyperlink ref="C26" r:id="rId62" xr:uid="{D25B05E4-FFE5-4DD1-8FA1-5AECD58245DF}"/>
+    <hyperlink ref="C27" r:id="rId63" xr:uid="{B03E9174-3F5D-41B9-BA5A-7D6CBECF5C3D}"/>
+    <hyperlink ref="C23" r:id="rId64" xr:uid="{6665C361-882B-4560-886D-DB46841737AF}"/>
+    <hyperlink ref="D9" r:id="rId65" xr:uid="{9F596094-4E2B-4F9E-B77B-993BE73D792B}"/>
+    <hyperlink ref="D10" r:id="rId66" xr:uid="{0CB543C9-8D4A-41BB-A6F0-749F082C6AB3}"/>
+    <hyperlink ref="D11" r:id="rId67" xr:uid="{1271D031-0FB6-4099-B514-4B320DE6AF6E}"/>
+    <hyperlink ref="D12" r:id="rId68" xr:uid="{24A3F74B-CB0A-4A1E-AD9E-101489BB6501}"/>
+    <hyperlink ref="D13" r:id="rId69" xr:uid="{1B3128E8-ED2C-4D63-ACB8-22F242620C78}"/>
+    <hyperlink ref="D14" r:id="rId70" xr:uid="{C8D60AEA-DBAE-4713-BF01-182AE815ADC9}"/>
+    <hyperlink ref="D15" r:id="rId71" xr:uid="{9FF73856-DAA9-42ED-A87A-6FF311822E61}"/>
+    <hyperlink ref="D16" r:id="rId72" xr:uid="{1F772B43-3F2B-4932-AC06-11442D7F162A}"/>
+    <hyperlink ref="D17" r:id="rId73" xr:uid="{D28EAA7F-2A7F-46F4-A152-404192C0FFFB}"/>
+    <hyperlink ref="D18" r:id="rId74" xr:uid="{EA6602BC-CB05-4B6B-B13A-14AD249068EA}"/>
+    <hyperlink ref="K4" r:id="rId75" xr:uid="{E42A79C5-65D2-42EE-B41D-CEB5F562F9CA}"/>
+    <hyperlink ref="K11" r:id="rId76" display="Ep 03" xr:uid="{0B55EA2C-47B0-4735-B621-C16CFE6287A2}"/>
+    <hyperlink ref="C36" r:id="rId77" xr:uid="{29D7B828-A9EC-497D-AC7C-A46FE3EE65A0}"/>
+    <hyperlink ref="K8" r:id="rId78" display="Get started with end-to-end analytics and lakehouses in Microsoft Fabric" xr:uid="{EE77E855-6A68-4E3B-9D05-28FAE3805576}"/>
+    <hyperlink ref="K10" r:id="rId79" xr:uid="{885D2ECA-8377-4615-8DB1-35576B77B6BD}"/>
+    <hyperlink ref="K7" r:id="rId80" display="Use Data Factory Pipelines in Microsoft Fabric" xr:uid="{F1812D9F-F687-42DC-9276-3A558D2863BB}"/>
+    <hyperlink ref="K5" r:id="rId81" xr:uid="{9412CDEC-897B-4A4B-945C-0BE9C458B9CA}"/>
+    <hyperlink ref="K15" r:id="rId82" display="Get started with data warehouses in Microsoft Fabric" xr:uid="{A56279AB-97D3-49D1-8576-DCF242657D94}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId83"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F180EED-F52E-41D2-8301-1E47E800243C}">
+  <dimension ref="B2:J43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -916,15 +2102,14 @@
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -952,18 +2137,15 @@
       <c r="J4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="33" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -984,11 +2166,8 @@
       <c r="J5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="26" t="s">
         <v>16</v>
@@ -1014,11 +2193,8 @@
       <c r="J6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="27" t="s">
         <v>27</v>
@@ -1044,15 +2220,12 @@
       <c r="J7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -1076,11 +2249,8 @@
       <c r="J8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="26" t="s">
         <v>12</v>
@@ -1106,11 +2276,8 @@
       <c r="J9" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="26" t="s">
         <v>13</v>
@@ -1136,11 +2303,8 @@
       <c r="J10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="26" t="s">
         <v>14</v>
@@ -1166,11 +2330,8 @@
       <c r="J11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="26" t="s">
         <v>29</v>
@@ -1196,11 +2357,8 @@
       <c r="J12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="26" t="s">
         <v>30</v>
@@ -1226,11 +2384,8 @@
       <c r="J13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="27" t="s">
         <v>15</v>
@@ -1256,18 +2411,15 @@
       <c r="J14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K14" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="33" t="s">
         <v>77</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1288,11 +2440,8 @@
       <c r="J15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="26" t="s">
         <v>8</v>
@@ -1318,11 +2467,8 @@
       <c r="J16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="26" t="s">
         <v>9</v>
@@ -1348,11 +2494,8 @@
       <c r="J17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="27" t="s">
         <v>10</v>
@@ -1378,15 +2521,12 @@
       <c r="J18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -1410,11 +2550,8 @@
       <c r="J19" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="26" t="s">
         <v>17</v>
@@ -1440,11 +2577,8 @@
       <c r="J20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K20" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="26" t="s">
         <v>20</v>
@@ -1470,11 +2604,8 @@
       <c r="J21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K21" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="27" t="s">
         <v>28</v>
@@ -1500,11 +2631,8 @@
       <c r="J22" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K22" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
@@ -1532,20 +2660,17 @@
       <c r="J23" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="26" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>41</v>
@@ -1562,11 +2687,8 @@
       <c r="J24" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="26" t="s">
         <v>19</v>
@@ -1592,11 +2714,8 @@
       <c r="J25" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K25" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="26" t="s">
         <v>31</v>
@@ -1622,11 +2741,8 @@
       <c r="J26" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K26" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="31" t="s">
         <v>57</v>
@@ -1652,11 +2768,8 @@
       <c r="J27" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>62</v>
       </c>
@@ -1684,11 +2797,8 @@
       <c r="J28" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="26" t="s">
         <v>22</v>
@@ -1714,11 +2824,8 @@
       <c r="J29" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="27" t="s">
         <v>23</v>
@@ -1744,131 +2851,116 @@
       <c r="J30" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K30" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="8" t="s">
+      <c r="F31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="J31" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="K31" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="4" t="s">
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="38"/>
+      <c r="C32" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I32" s="5" t="s">
+      <c r="F32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="K32" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="20" t="s">
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="38"/>
+      <c r="C33" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H33" s="5" t="s">
+      <c r="D33" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="K33" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="21" t="s">
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="43"/>
+      <c r="C34" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I34" s="6" t="s">
+      <c r="F34" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="J34" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="K34" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>84</v>
       </c>
@@ -1879,7 +2971,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>85</v>
       </c>
@@ -1890,7 +2982,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>97</v>
       </c>
@@ -1898,7 +2990,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>54</v>
       </c>
@@ -1909,7 +3001,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>55</v>
       </c>
@@ -1920,7 +3012,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>100</v>
       </c>
@@ -1928,7 +3020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>63</v>
       </c>
@@ -1939,13 +3031,13 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B4:K34" xr:uid="{3F180EED-F52E-41D2-8301-1E47E800243C}"/>
+  <autoFilter ref="B4:J34" xr:uid="{3F180EED-F52E-41D2-8301-1E47E800243C}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4BF04D53-5D6A-4C00-85EE-51A4DB2B216B}"/>
     <hyperlink ref="B15" r:id="rId2" xr:uid="{D822AA2C-BA0B-41C9-8934-FF810D4F97E9}"/>
@@ -2021,31 +3113,17 @@
     <hyperlink ref="D16" r:id="rId72" xr:uid="{3AA2ACF9-071B-40FD-ADA7-E5BFE6974B15}"/>
     <hyperlink ref="D17" r:id="rId73" xr:uid="{A20AF6BF-DF5A-41F4-AC10-F0F04C6BFC03}"/>
     <hyperlink ref="D18" r:id="rId74" xr:uid="{DD08DC7F-0591-48A5-A6D0-C06F6E7EEEB0}"/>
-    <hyperlink ref="K5" r:id="rId75" xr:uid="{6F9E5C26-8A97-4E93-9CB4-EF80B6EF11FE}"/>
-    <hyperlink ref="K7" r:id="rId76" xr:uid="{F2A84E33-E84D-4DD0-9626-5E3F2BB758CA}"/>
-    <hyperlink ref="K31" r:id="rId77" xr:uid="{2111E2F7-9B2C-414C-A004-571CEE18CA6C}"/>
-    <hyperlink ref="K10" r:id="rId78" xr:uid="{6FE93CA3-CD97-43E6-93A3-5AC135D9B844}"/>
-    <hyperlink ref="K11" r:id="rId79" xr:uid="{F34FD9F6-1274-4312-B4AF-748230F070D3}"/>
-    <hyperlink ref="K33" r:id="rId80" xr:uid="{E7D1FF3E-56EC-4F77-B8F4-991A4C58E718}"/>
-    <hyperlink ref="K32" r:id="rId81" xr:uid="{98429706-550E-4099-8091-C34AF75A02BD}"/>
-    <hyperlink ref="K15" r:id="rId82" xr:uid="{DC45D908-5BE3-4615-9007-47B4C73E1D1F}"/>
-    <hyperlink ref="K8" r:id="rId83" xr:uid="{DDDE61A0-B00D-4825-A108-6BD901BE9948}"/>
-    <hyperlink ref="K4" r:id="rId84" xr:uid="{7A69C6A0-BEF6-44B2-8072-0D5669F6838B}"/>
-    <hyperlink ref="K12" r:id="rId85" xr:uid="{CAF6D0F6-D6A4-4B73-BD2B-F80785B04D99}"/>
-    <hyperlink ref="K13" r:id="rId86" xr:uid="{977C48C1-72B8-4F98-A3CC-BAC2FEE2E9D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId87"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A18723-27DE-4F05-A927-2EE537C61CF1}">
   <dimension ref="B2:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2099,10 +3177,10 @@
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="33" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -2182,7 +3260,7 @@
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -2373,10 +3451,10 @@
       <c r="B15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="33" t="s">
         <v>77</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -2483,7 +3561,7 @@
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -2624,10 +3702,10 @@
         <v>18</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>41</v>
@@ -2727,7 +3805,7 @@
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="26" t="s">
@@ -2810,110 +3888,110 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J31" s="13" t="s">
+      <c r="F31" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="46" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="38"/>
+      <c r="C32" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32" s="12" t="s">
+      <c r="F32" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" s="47" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="20" t="s">
+      <c r="B33" s="38"/>
+      <c r="C33" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J33" s="12" t="s">
+      <c r="D33" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="47" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="43"/>
+      <c r="C34" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J34" s="15" t="s">
+      <c r="F34" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="J34" s="48" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>